<commit_message>
excel tabelki z obliczeniami
</commit_message>
<xml_diff>
--- a/Sprawozdanie 3/Excel.xlsx
+++ b/Sprawozdanie 3/Excel.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Miedź" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="19">
   <si>
     <t>Nr harmonicznej</t>
   </si>
@@ -107,12 +107,57 @@
       <t>[m/s]</t>
     </r>
   </si>
+  <si>
+    <t>Średnia prędkość fali</t>
+  </si>
+  <si>
+    <t>błąd bezwzględny</t>
+  </si>
+  <si>
+    <t>Sp</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>l [m]</t>
+  </si>
+  <si>
+    <t>d [m]</t>
+  </si>
+  <si>
+    <t>dw [m]</t>
+  </si>
+  <si>
+    <t>m [kg]</t>
+  </si>
+  <si>
+    <t>ro</t>
+  </si>
+  <si>
+    <t>h [m]</t>
+  </si>
+  <si>
+    <t>Pp</t>
+  </si>
+  <si>
+    <t>a [m]</t>
+  </si>
+  <si>
+    <t>b [m]</t>
+  </si>
+  <si>
+    <t>c [m]</t>
+  </si>
+  <si>
+    <t>Young</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -151,6 +196,13 @@
       <family val="2"/>
       <charset val="238"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -172,7 +224,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -183,6 +235,10 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -463,18 +519,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="4" width="15.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" customWidth="1"/>
+    <col min="13" max="13" width="13.42578125" customWidth="1"/>
+    <col min="14" max="14" width="11.85546875" customWidth="1"/>
+    <col min="15" max="15" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -487,8 +547,35 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -499,12 +586,44 @@
         <f>3.6/A2</f>
         <v>3.6</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="4">
         <f>C2*B2</f>
         <v>4248</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F2">
+        <f>AVERAGE(D3:D7)</f>
+        <v>3827.04</v>
+      </c>
+      <c r="G2">
+        <f>ABS(D2-$F$2)</f>
+        <v>420.96000000000004</v>
+      </c>
+      <c r="I2">
+        <v>1.52E-2</v>
+      </c>
+      <c r="J2">
+        <v>1.7950000000000001E-2</v>
+      </c>
+      <c r="K2" s="5">
+        <v>1.8009999999999999</v>
+      </c>
+      <c r="L2">
+        <v>0.76100000000000001</v>
+      </c>
+      <c r="M2">
+        <f>(PI()/4)*((J2^2)-(I2^2))</f>
+        <v>7.1598860070719872E-5</v>
+      </c>
+      <c r="N2">
+        <f>M2*K2</f>
+        <v>1.2894954698736648E-4</v>
+      </c>
+      <c r="O2">
+        <f>L2/N2</f>
+        <v>5901.5329466380917</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <f>A2+1</f>
         <v>2</v>
@@ -520,10 +639,14 @@
         <f t="shared" ref="D3:D7" si="1">C3*B3</f>
         <v>3888</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G3">
+        <f t="shared" ref="G3:G7" si="2">ABS(D3-$F$2)</f>
+        <v>60.960000000000036</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <f t="shared" ref="A4:A7" si="2">A3+1</f>
+        <f t="shared" ref="A4:A7" si="3">A3+1</f>
         <v>3</v>
       </c>
       <c r="B4" s="1">
@@ -537,10 +660,14 @@
         <f t="shared" si="1"/>
         <v>3888</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G4">
+        <f t="shared" si="2"/>
+        <v>60.960000000000036</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="B5" s="1">
@@ -554,10 +681,17 @@
         <f t="shared" si="1"/>
         <v>3852</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G5">
+        <f t="shared" si="2"/>
+        <v>24.960000000000036</v>
+      </c>
+      <c r="J5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="B6" s="1">
@@ -571,10 +705,18 @@
         <f t="shared" si="1"/>
         <v>3787.2</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G6">
+        <f t="shared" si="2"/>
+        <v>39.840000000000146</v>
+      </c>
+      <c r="J6">
+        <f>O2*F2^2</f>
+        <v>86435239350.391678</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="B7" s="1">
@@ -587,6 +729,10 @@
       <c r="D7" s="1">
         <f t="shared" si="1"/>
         <v>3720</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="2"/>
+        <v>107.03999999999996</v>
       </c>
     </row>
   </sheetData>
@@ -597,18 +743,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D7"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="4" width="15.28515625" customWidth="1"/>
+    <col min="10" max="10" width="10" customWidth="1"/>
+    <col min="12" max="13" width="12" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -621,8 +770,32 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -637,8 +810,37 @@
         <f>C2*B2</f>
         <v>4821.3</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F2">
+        <f>AVERAGE(D2:D6)</f>
+        <v>4696.0320000000002</v>
+      </c>
+      <c r="G2">
+        <f>ABS(D2-$F$2)</f>
+        <v>125.26800000000003</v>
+      </c>
+      <c r="I2">
+        <v>0.33900000000000002</v>
+      </c>
+      <c r="J2">
+        <v>4.8999999999999998E-3</v>
+      </c>
+      <c r="K2">
+        <v>2.4E-2</v>
+      </c>
+      <c r="L2">
+        <f>(PI()/4)*J2^2</f>
+        <v>1.8857409903172734E-5</v>
+      </c>
+      <c r="M2">
+        <f>I2*L2</f>
+        <v>6.3926619571755575E-6</v>
+      </c>
+      <c r="N2">
+        <f>K2/M2</f>
+        <v>3754.3045699547388</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <f>A2+1</f>
         <v>2</v>
@@ -654,10 +856,14 @@
         <f t="shared" ref="D3:D7" si="1">C3*B3</f>
         <v>4920.3</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G3">
+        <f t="shared" ref="G3:G7" si="2">ABS(D3-$F$2)</f>
+        <v>224.26800000000003</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <f t="shared" ref="A4:A7" si="2">A3+1</f>
+        <f t="shared" ref="A4:A7" si="3">A3+1</f>
         <v>3</v>
       </c>
       <c r="B4" s="1">
@@ -671,10 +877,14 @@
         <f t="shared" si="1"/>
         <v>4515.72</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G4">
+        <f t="shared" si="2"/>
+        <v>180.3119999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="B5" s="1">
@@ -688,10 +898,17 @@
         <f t="shared" si="1"/>
         <v>4732.2</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G5">
+        <f t="shared" si="2"/>
+        <v>36.167999999999665</v>
+      </c>
+      <c r="J5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="B6" s="1">
@@ -705,10 +922,18 @@
         <f t="shared" si="1"/>
         <v>4490.6400000000003</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G6">
+        <f t="shared" si="2"/>
+        <v>205.39199999999983</v>
+      </c>
+      <c r="J6">
+        <f>N2*F2^2</f>
+        <v>82792614504.900085</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="B7" s="1">
@@ -718,9 +943,13 @@
         <f t="shared" si="0"/>
         <v>0.33</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="4">
         <f t="shared" si="1"/>
         <v>4082.1000000000004</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="2"/>
+        <v>613.93199999999979</v>
       </c>
     </row>
   </sheetData>
@@ -730,18 +959,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:N7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="4" width="15.42578125" customWidth="1"/>
+    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -754,8 +985,32 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -770,8 +1025,37 @@
         <f>C2*B2</f>
         <v>3346.2</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F2">
+        <f>AVERAGE(D2:D6)</f>
+        <v>3398.076</v>
+      </c>
+      <c r="G2">
+        <f>ABS(D2-$F$2)</f>
+        <v>51.876000000000204</v>
+      </c>
+      <c r="I2">
+        <v>0.311</v>
+      </c>
+      <c r="J2">
+        <v>5.8999999999999999E-3</v>
+      </c>
+      <c r="K2">
+        <v>7.3999999999999996E-2</v>
+      </c>
+      <c r="L2">
+        <f>(PI()/4)*J2^2</f>
+        <v>2.7339710067865173E-5</v>
+      </c>
+      <c r="M2">
+        <f>I2*L2</f>
+        <v>8.5026498311060694E-6</v>
+      </c>
+      <c r="N2">
+        <f>K2/M2</f>
+        <v>8703.1691848908813</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <f>A2+1</f>
         <v>2</v>
@@ -787,10 +1071,14 @@
         <f t="shared" ref="D3:D7" si="1">C3*B3</f>
         <v>3435.3</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G3">
+        <f t="shared" ref="G3:G7" si="2">ABS(D3-$F$2)</f>
+        <v>37.22400000000016</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <f t="shared" ref="A4:A7" si="2">A3+1</f>
+        <f t="shared" ref="A4:A7" si="3">A3+1</f>
         <v>3</v>
       </c>
       <c r="B4" s="1">
@@ -804,10 +1092,14 @@
         <f t="shared" si="1"/>
         <v>3405.6000000000004</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G4">
+        <f t="shared" si="2"/>
+        <v>7.524000000000342</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="B5" s="1">
@@ -821,10 +1113,17 @@
         <f t="shared" si="1"/>
         <v>3385.8</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G5">
+        <f t="shared" si="2"/>
+        <v>12.27599999999984</v>
+      </c>
+      <c r="J5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="B6" s="1">
@@ -838,10 +1137,18 @@
         <f t="shared" si="1"/>
         <v>3417.48</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G6">
+        <f t="shared" si="2"/>
+        <v>19.403999999999996</v>
+      </c>
+      <c r="J6">
+        <f>N2*F2^2</f>
+        <v>100494802691.44164</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="B7" s="1">
@@ -851,9 +1158,13 @@
         <f t="shared" si="0"/>
         <v>0.33</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="4">
         <f t="shared" si="1"/>
         <v>3960</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="2"/>
+        <v>561.92399999999998</v>
       </c>
     </row>
   </sheetData>
@@ -863,18 +1174,21 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="4" width="15.42578125" customWidth="1"/>
+    <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -887,8 +1201,32 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -903,8 +1241,36 @@
         <f>C2*B2</f>
         <v>5076</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F2">
+        <f>SUM(D2:D7)/A7</f>
+        <v>5150.4000000000005</v>
+      </c>
+      <c r="G2">
+        <f>ABS(D2-$F$2)</f>
+        <v>74.400000000000546</v>
+      </c>
+      <c r="I2">
+        <v>1.9E-2</v>
+      </c>
+      <c r="J2">
+        <v>1.41E-2</v>
+      </c>
+      <c r="K2">
+        <v>1.4200000000000001E-2</v>
+      </c>
+      <c r="L2">
+        <v>3.1859999999999999E-2</v>
+      </c>
+      <c r="M2">
+        <f>I2*J2*K2</f>
+        <v>3.8041800000000002E-6</v>
+      </c>
+      <c r="N2">
+        <f>L2/M2</f>
+        <v>8374.9980284844551</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <f>A2+1</f>
         <v>2</v>
@@ -920,10 +1286,14 @@
         <f t="shared" ref="D3:D7" si="1">C3*B3</f>
         <v>5220</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G3">
+        <f t="shared" ref="G3:G7" si="2">ABS(D3-$F$2)</f>
+        <v>69.599999999999454</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <f t="shared" ref="A4:A7" si="2">A3+1</f>
+        <f t="shared" ref="A4:A7" si="3">A3+1</f>
         <v>3</v>
       </c>
       <c r="B4" s="1">
@@ -937,10 +1307,14 @@
         <f t="shared" si="1"/>
         <v>5172</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G4">
+        <f t="shared" si="2"/>
+        <v>21.599999999999454</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="B5" s="1">
@@ -954,10 +1328,17 @@
         <f t="shared" si="1"/>
         <v>5148</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G5">
+        <f t="shared" si="2"/>
+        <v>2.4000000000005457</v>
+      </c>
+      <c r="J5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="B6" s="1">
@@ -971,10 +1352,18 @@
         <f t="shared" si="1"/>
         <v>5126.3999999999996</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G6">
+        <f t="shared" si="2"/>
+        <v>24.000000000000909</v>
+      </c>
+      <c r="J6">
+        <f>N2*F2^2</f>
+        <v>222160391542.35602</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="B7" s="1">
@@ -987,6 +1376,10 @@
       <c r="D7" s="1">
         <f t="shared" si="1"/>
         <v>5160</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="2"/>
+        <v>9.5999999999994543</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tabelki z obliczeniami wszystkimi
</commit_message>
<xml_diff>
--- a/Sprawozdanie 3/Excel.xlsx
+++ b/Sprawozdanie 3/Excel.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Miedź" sheetId="1" r:id="rId1"/>
@@ -521,8 +521,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -579,7 +579,7 @@
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="4">
         <v>1180</v>
       </c>
       <c r="C2" s="3">
@@ -746,7 +746,7 @@
   <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -936,7 +936,7 @@
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="4">
         <v>12370</v>
       </c>
       <c r="C7" s="3">
@@ -961,8 +961,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1151,7 +1151,7 @@
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="4">
         <v>12000</v>
       </c>
       <c r="C7" s="3">

</xml_diff>

<commit_message>
Poprawiona masa próbki stalowej
</commit_message>
<xml_diff>
--- a/Sprawozdanie 3/Excel.xlsx
+++ b/Sprawozdanie 3/Excel.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Miedź" sheetId="1" r:id="rId1"/>
@@ -521,7 +521,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -1176,8 +1176,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1259,7 +1259,7 @@
         <v>1.4200000000000001E-2</v>
       </c>
       <c r="L2">
-        <v>3.1859999999999999E-2</v>
+        <v>3.0859999999999999E-2</v>
       </c>
       <c r="M2">
         <f>I2*J2*K2</f>
@@ -1267,7 +1267,7 @@
       </c>
       <c r="N2">
         <f>L2/M2</f>
-        <v>8374.9980284844551</v>
+        <v>8112.1292893606496</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -1358,7 +1358,7 @@
       </c>
       <c r="J6">
         <f>N2*F2^2</f>
-        <v>222160391542.35602</v>
+        <v>215187372347.68073</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">

</xml_diff>